<commit_message>
pushing school data live
</commit_message>
<xml_diff>
--- a/static/life.xlsx
+++ b/static/life.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qasim/NodeJs/givezakat/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65854BDF-9D6D-2742-8692-464C11C3E029}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CBD4EA3-B1A8-8D49-AFC9-4E1258C2B119}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
   </bookViews>
@@ -574,24 +574,6 @@
     <t>STQA</t>
   </si>
   <si>
-    <t>Topic: name- Week 1,lectures- 1 Lecture, duration- 00:00;
-Slides: slide- Chapter1.pptx;</t>
-  </si>
-  <si>
-    <t>Subject: Advanced Theory of Computation;
-Instructor: Dr Ali Arshad;
-ClassSenior: +92 313 7408286;
-Note: This website is going premium in 3 to 4 days. You can register yourself by contacting Qasim at Rs 350 / month or Rs 1400 / course. In this payment all courses will be open.;
-CreditHours: 3.0;</t>
-  </si>
-  <si>
-    <t>Subject: Software Testing and Quality Assurance;
-Instructor: Dr Abdul Hannan;
-ClassSenior: N/A;
-Note: This website is going premium in 3 to 4 days. You can register yourself by contacting Qasim at Rs 350 / month or Rs 1400 one time / course duration. In this payment all courses will be open.;
-CreditHours: 3.0;</t>
-  </si>
-  <si>
     <t>Topic: name- Week 1,lectures- 1 Lecture, duration- 01:37;
 Video: link- https://drive.google.com/file/d/1YOq3u1x-LfM-TkOvDmc8IIrJ3l2MCywy/preview, name- AOS Week#1part1.mp4, duration- 01:09;
 Video: link- https://drive.google.com/file/d/1Nh8zm9SXHbo87Ge5tT8hdPpfrUb1AlaK/preview, name- AOS Week#1part2.mp4, duration- 00:28;
@@ -600,8 +582,29 @@
   <si>
     <t>Subject: Advanced Operating System;
 Instructor: Dr Nasir Mehmood;
+ClassSenior: Awais, +92 323 7800196;
+Note: Stay tuned for updates.;
+CreditHours: 3.0;</t>
+  </si>
+  <si>
+    <t>Subject: Advanced Theory of Computation;
+Instructor: Dr Ali Arshad;
+ClassSenior: +92 313 7408286;
+Note:  Stay tuned for updates.;
+CreditHours: 3.0;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Topic: name- Week 1,lectures- 1 Lecture, duration- 00:00;
+Slides: slide- Chapter1.pptx;
+Assignment: name- Assignment 1 (Deadline 1st Feb 2020), img- /STQA/Assignment 1.png;
+Note: heading- Submit assignment if you are late. Sir might accept it. I also have not done it yet.;
+</t>
+  </si>
+  <si>
+    <t>Subject: Software Testing and Quality Assurance;
+Instructor: Dr Abdul Hannan;
 ClassSenior: N/A;
-Note: This website is going premium in 3 to 4 days. You can register yourself by contacting Qasim at Rs 350 / month or Rs 1400 one time / course duration. In this payment all courses will be open.;
+Note: Stay tuned for updates.;
 CreditHours: 3.0;</t>
   </si>
 </sst>
@@ -1019,8 +1022,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05FB8366-CFB7-BD41-BAF1-2BC53FC93C19}">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F2" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1066,7 +1069,7 @@
       </c>
       <c r="N1" s="6"/>
     </row>
-    <row r="2" spans="1:14" ht="136" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" ht="119" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>27</v>
       </c>
@@ -1084,13 +1087,13 @@
         <v>49</v>
       </c>
       <c r="G2" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="H2" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="I2" s="14" t="s">
         <v>86</v>
-      </c>
-      <c r="I2" s="14" t="s">
-        <v>84</v>
       </c>
       <c r="J2" s="14"/>
       <c r="N2" s="6"/>
@@ -1116,10 +1119,10 @@
         <v>78</v>
       </c>
       <c r="H3" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="I3" s="14" t="s">
         <v>85</v>
-      </c>
-      <c r="I3" s="14" t="s">
-        <v>82</v>
       </c>
       <c r="N3" s="6"/>
     </row>

</xml_diff>

<commit_message>
course updated for ATOC and AOS
</commit_message>
<xml_diff>
--- a/static/life.xlsx
+++ b/static/life.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/QasimAli/nodejs/givezakat/static/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qasim/NodeJs/givezakat/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E4BEFEE-628E-8E47-BCB1-31AC1F780D0D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40F98051-BC60-0240-B45F-B11340F44AB8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35800" windowHeight="18000" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16740" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="91">
   <si>
     <t>Algo</t>
   </si>
@@ -557,11 +557,6 @@
     <t>ATOC</t>
   </si>
   <si>
-    <t>Topic: name- Week 2,lectures- 1 Lecture, duration- 01:44;
-Video: link- https://drive.google.com/file/d/1LLPqYvPSZruiDnWQfo4C6cxPAwNAJBAc/preview, name- ATC Week#2, duration- 01:44;
-Slides: slide- Lec1.pdf;</t>
-  </si>
-  <si>
     <t>AOS</t>
   </si>
   <si>
@@ -595,17 +590,6 @@
 Slides: slide- Chapter 2.ppt;</t>
   </si>
   <si>
-    <t>Topic: name- Week 2,lectures- 1 Lecture, duration- 01:33;
-Video: link- https://drive.google.com/file/d/18qBlYxrN38HZh1pjIysBGtg8SF1JSLY0/preview, name- AOS Week#1part1.mp4, duration- 01:33;
-Slides: slide- Chapter 3.ppt;</t>
-  </si>
-  <si>
-    <t>Topic: name- Week 3,lectures- 2 Lectures, duration- 01:49;
-Video: link- https://drive.google.com/file/d/15puMyWTcN0p2nEstcIl5CfRdY9_QJMQ9/preview, name- ATC Week#3, duration- 00:31;
-Video: link- https://drive.google.com/file/d/1LHMHVg2vCtKk4WZw6evB8Ly6JOxUGj8X/preview, name- ATC Week#3, duration- 01:18;
-Slides: slide- Lec1.pdf;</t>
-  </si>
-  <si>
     <t>Subject: Advanced Theory of Computation;
 Instructor: Dr Ali Arshad;
 ClassSenior: Hassan, +92 313 7408286;
@@ -613,8 +597,35 @@
 CreditHours: 3.0;</t>
   </si>
   <si>
+    <t>Topic: name- Week 2,lectures- 1 Lecture, duration- 01:33;
+Video: link- https://drive.google.com/file/d/18qBlYxrN38HZh1pjIysBGtg8SF1JSLY0/preview, name- AOS Week#2part1.mp4, duration- 01:33;
+Slides: slide- Chapter 3.ppt;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 3,lectures- 2 Lectures, duration- 01:38;
+Video: link- https://drive.google.com/file/d/1CEA0dNMZFnAwwcInBt37frFSakNJSyuO/preview, name- AOS Week#3part1.mp4, duration- 01:06;
+Video: link- https://drive.google.com/file/d/19aBooNe8gvSiXqm-yxEMN2AHg0KthhYP/preview, name- AOS Week#3part2.mp4, duration- 00:32;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 4,lectures- 3 Lectures, duration- 01:40;
+Video: link- https://drive.google.com/file/d/1dWC0HSI8lJ4ASxDgWuTYJ3bl1GrZ-Z-5/preview, name- ATOC Week#4Part1.mp4, duration- 00:50;
+Video: link- https://drive.google.com/file/d/1qLxWUU9e9HeNY8DNLhalPa_CQbaxo8k_/preview, name- ATOC Week#4Part2.mp4, duration- 00:48;
+Video: link- https://drive.google.com/file/d/1ZKP1-pdg6o_ifZ4GOkHRCjUUrnaqArza/preview, name- ATOC Week#4Part3.mp4, duration- 00:02;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 3,lectures- 2 Lectures, duration- 01:49;
+Video: link- https://drive.google.com/file/d/15puMyWTcN0p2nEstcIl5CfRdY9_QJMQ9/preview, name- ATC Week#3Part1.mp4, duration- 00:31;
+Video: link- https://drive.google.com/file/d/1LHMHVg2vCtKk4WZw6evB8Ly6JOxUGj8X/preview, name- ATC Week#3Part2.mp4, duration- 01:18;
+Slides: slide- Lec1.pdf;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 2,lectures- 1 Lecture, duration- 01:44;
+Video: link- https://drive.google.com/file/d/1LLPqYvPSZruiDnWQfo4C6cxPAwNAJBAc/preview, name- ATC Week#2.mp4, duration- 01:44;
+Slides: slide- Lec1.pdf;</t>
+  </si>
+  <si>
     <t>Topic: name- Week 1,lectures- 1 Lecture, duration- 01:20;
-Video: link- https://drive.google.com/file/d/19dipmMmEiCQmlntPtJAtKF_DfoD_sufk/preview, name- ATC Week#1, duration- 01:20;
+Video: link- https://drive.google.com/file/d/19dipmMmEiCQmlntPtJAtKF_DfoD_sufk/preview, name- ATC Week#1.mp4, duration- 01:20;
 Slides: slide- Course.pdf;
 Slides: slide- Lec1.pdf;
 Topics: Finite state machine, Applications of Finite Automata, Proving techniques</t>
@@ -1037,8 +1048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05FB8366-CFB7-BD41-BAF1-2BC53FC93C19}">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E3" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="F6" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1077,10 +1088,10 @@
         <v>77</v>
       </c>
       <c r="H1" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="I1" s="12" t="s">
         <v>79</v>
-      </c>
-      <c r="I1" s="12" t="s">
-        <v>80</v>
       </c>
       <c r="N1" s="6"/>
     </row>
@@ -1102,13 +1113,13 @@
         <v>49</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I2" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J2" s="14"/>
       <c r="N2" s="6"/>
@@ -1131,13 +1142,13 @@
         <v>50</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I3" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="N3" s="6"/>
     </row>
@@ -1157,7 +1168,7 @@
       </c>
       <c r="F4" s="14"/>
       <c r="G4" s="14" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="H4" s="15" t="s">
         <v>85</v>
@@ -1179,6 +1190,9 @@
         <v>32</v>
       </c>
       <c r="G5" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="H5" s="15" t="s">
         <v>86</v>
       </c>
       <c r="N5" s="5"/>
@@ -1197,6 +1211,9 @@
       <c r="E6" s="14" t="s">
         <v>34</v>
       </c>
+      <c r="G6" s="14" t="s">
+        <v>87</v>
+      </c>
       <c r="N6" s="5"/>
     </row>
     <row r="7" spans="1:14" ht="323" x14ac:dyDescent="0.2">
@@ -1233,7 +1250,7 @@
       </c>
       <c r="F8" s="10"/>
     </row>
-    <row r="9" spans="1:14" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A9" s="8">
         <v>43775</v>
       </c>

</xml_diff>

<commit_message>
Updated course for all subjects
</commit_message>
<xml_diff>
--- a/static/life.xlsx
+++ b/static/life.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/QasimAli/nodejs/givezakat/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C33266A-438C-754A-8390-9123818B9338}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACE1C66D-97DD-D147-9BF2-BD3C68F7DDEF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16740" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="100">
   <si>
     <t>Algo</t>
   </si>
@@ -662,6 +662,33 @@
     <t>Topic: name- Week 5, lectures- 2 Lectures, duration- 01:09;
 Video: link- https://drive.google.com/file/d/1p65AFQnFqjgadbb6Z6iOBRrxk4hrAPYU/preview, name- AOS Week5part1.mp4, duration- 01:01;
 Video: link- https://drive.google.com/file/d/1v73JQCmN0GASJYm3syH_MdRRcuVtO8kM/preview, name- AOS Week#5part2.mp4, duration- 00:08;</t>
+  </si>
+  <si>
+    <t>Topic: name- Mid Term Exam, lectures- , duration-  13 Mar | 15:00-16:30;
+Assignment: name- Course for Mid Term, img- /ATOC/course.jpeg;
+Slides: slide- Course.pdf;
+Slides: slide- Lec1.pdf;
+Note: heading- Watch all lectures taught in class to prepare for exams;</t>
+  </si>
+  <si>
+    <t>Topic: name- Mid Term Exam, lectures- , duration-  14 Mar | 11:00-12:30;
+Assignment: name- Course for Mid Term, img- /AOS/course.jpeg;
+Slides: slide- Chapter1.pptx;
+Slides: slide- Chapter2.pptx;
+Slides: slide- Chapter3.ppt;
+Slides: slide- Paper No 1.pdf;
+Slides: slide- Paper No 2.pdf;
+Slides: slide- Paper No 3.pdf;
+Note: heading- Prepare all lectures pasted above. Must read book. I do not have yet. I will share as I get it.;</t>
+  </si>
+  <si>
+    <t>Topic: name- Mid Term Exam, lectures- , duration-  15 Mar | 11:00-12:30;
+Assignment: name- Course for Mid Term, img- /AOS/course.jpeg;
+Slides: slide- Chapter 1.ppt;
+Slides: slide- Chapter 2.ppt;
+Slides: slide- Chapter 3.ppt;
+Assignment: name- Picture of Board, img- /AOS/board.jpeg;
+Note: heading- Prepare all lectures pasted above.;</t>
   </si>
 </sst>
 </file>
@@ -1081,8 +1108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05FB8366-CFB7-BD41-BAF1-2BC53FC93C19}">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E4" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="G7" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1256,6 +1283,9 @@
       <c r="H6" s="15" t="s">
         <v>95</v>
       </c>
+      <c r="I6" s="14" t="s">
+        <v>98</v>
+      </c>
       <c r="N6" s="5"/>
     </row>
     <row r="7" spans="1:14" ht="323" x14ac:dyDescent="0.2">
@@ -1299,6 +1329,9 @@
       <c r="G8" s="14" t="s">
         <v>91</v>
       </c>
+      <c r="H8" s="14" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="9" spans="1:14" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A9" s="8">
@@ -1313,6 +1346,9 @@
       </c>
       <c r="E9" s="14" t="s">
         <v>53</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="238" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
updated course for stqa and ATOC
</commit_message>
<xml_diff>
--- a/static/life.xlsx
+++ b/static/life.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/QasimAli/nodejs/givezakat/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AA7DEF5-03F4-964A-8517-D1DE11379B24}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F00F231-325B-CA41-B308-853D2A83D749}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16740" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -602,36 +602,11 @@
 Slides: slide- Chapter 3.ppt;</t>
   </si>
   <si>
-    <t>Topic: name- Week 4,lectures- 3 Lectures, duration- 01:40;
-Video: link- https://drive.google.com/file/d/1dWC0HSI8lJ4ASxDgWuTYJ3bl1GrZ-Z-5/preview, name- ATOC Week#4Part1.mp4, duration- 00:50;
-Video: link- https://drive.google.com/file/d/1qLxWUU9e9HeNY8DNLhalPa_CQbaxo8k_/preview, name- ATOC Week#4Part2.mp4, duration- 00:48;
-Video: link- https://drive.google.com/file/d/1ZKP1-pdg6o_ifZ4GOkHRCjUUrnaqArza/preview, name- ATOC Week#4Part3.mp4, duration- 00:02;</t>
-  </si>
-  <si>
-    <t>Topic: name- Week 3,lectures- 2 Lectures, duration- 01:49;
-Video: link- https://drive.google.com/file/d/15puMyWTcN0p2nEstcIl5CfRdY9_QJMQ9/preview, name- ATC Week#3Part1.mp4, duration- 00:31;
-Video: link- https://drive.google.com/file/d/1LHMHVg2vCtKk4WZw6evB8Ly6JOxUGj8X/preview, name- ATC Week#3Part2.mp4, duration- 01:18;
-Slides: slide- Lec1.pdf;</t>
-  </si>
-  <si>
-    <t>Topic: name- Week 2,lectures- 1 Lecture, duration- 01:44;
-Video: link- https://drive.google.com/file/d/1LLPqYvPSZruiDnWQfo4C6cxPAwNAJBAc/preview, name- ATC Week#2.mp4, duration- 01:44;
-Slides: slide- Lec1.pdf;</t>
-  </si>
-  <si>
     <t>Topic: name- Week 1,lectures- 1 Lecture, duration- 01:20;
 Video: link- https://drive.google.com/file/d/19dipmMmEiCQmlntPtJAtKF_DfoD_sufk/preview, name- ATC Week#1.mp4, duration- 01:20;
 Slides: slide- Course.pdf;
 Slides: slide- Lec1.pdf;
 Topics: Finite state machine, Applications of Finite Automata, Proving techniques</t>
-  </si>
-  <si>
-    <t>Topic: name- Week 5, lectures- 4 Lectures, duration- 01:23;
-Video: link- https://drive.google.com/file/d/1MFTDv0iYQzWbW_4VCX7PgDr3-UYf4800/preview, name- ATOC Week#5Part1.mp4, duration- 00:27;
-Video: link- https://drive.google.com/file/d/17RximV5JzVFI3eu-9ir6eFv8s_kbdfAe/preview, name- ATOC Week#5Part2.mp4, duration- 00:01;
-Video: link- https://drive.google.com/file/d/1pSGNEYEJkci8ely09oc-rdTtnI2ljeqE/preview, name- ATOC Week#5Part3.mp4, duration- 00:53;
-Video: link- https://drive.google.com/file/d/1NJH2YpnIsmDwipOJSgILBo_Ta0u6klH4/preview, name- ATOC Week#5Part4.mp4, duration- 00:02;
-Note: heading- Presentation in next class;</t>
   </si>
   <si>
     <t>Topic: name- Week 6, lectures- 3 Lectures, duration- 01:34;
@@ -673,22 +648,56 @@
 Note: heading- Prepare all lectures pasted above.;</t>
   </si>
   <si>
+    <t>Topic: name- Mid Term Exam, lectures- , duration-  13 Mar | 15:00-16:30;
+Assignment: name- Course for Mid Term, img- /ATOC/Course.jpeg;
+Slides: slide- Course.pdf;
+Slides: slide- Lec1.pdf;
+Note: heading- Watch all lectures taught in class to prepare for exams;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 2,lectures- 1 Lecture, duration- 01:44;
+Video: link- https://drive.google.com/file/d/1LLPqYvPSZruiDnWQfo4C6cxPAwNAJBAc/preview, name- ATC Week#2.mp4, duration- 01:44;
+Slides: slide- Lec1.pdf;
+Topics: Constructing DFA;
+Note: heading- Write research paper on your favorite article;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 3,lectures- 2 Lectures, duration- 01:49;
+Video: link- https://drive.google.com/file/d/15puMyWTcN0p2nEstcIl5CfRdY9_QJMQ9/preview, name- ATC Week#3Part1.mp4, duration- 00:31;
+Video: link- https://drive.google.com/file/d/1LHMHVg2vCtKk4WZw6evB8Ly6JOxUGj8X/preview, name- ATC Week#3Part2.mp4, duration- 01:18;
+Slides: slide- Lec1.pdf;
+Topics: Constructing NFA;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 4,lectures- 3 Lectures, duration- 01:40;
+Video: link- https://drive.google.com/file/d/1dWC0HSI8lJ4ASxDgWuTYJ3bl1GrZ-Z-5/preview, name- ATOC Week#4Part1.mp4, duration- 00:50;
+Video: link- https://drive.google.com/file/d/1qLxWUU9e9HeNY8DNLhalPa_CQbaxo8k_/preview, name- ATOC Week#4Part2.mp4, duration- 00:48;
+Video: link- https://drive.google.com/file/d/1ZKP1-pdg6o_ifZ4GOkHRCjUUrnaqArza/preview, name- ATOC Week#4Part3.mp4, duration- 00:02;
+Topics: Conversion of NFA to DFA;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 5, lectures- 4 Lectures, duration- 01:23;
+Video: link- https://drive.google.com/file/d/1MFTDv0iYQzWbW_4VCX7PgDr3-UYf4800/preview, name- ATOC Week#5Part1.mp4, duration- 00:27;
+Video: link- https://drive.google.com/file/d/17RximV5JzVFI3eu-9ir6eFv8s_kbdfAe/preview, name- ATOC Week#5Part2.mp4, duration- 00:01;
+Video: link- https://drive.google.com/file/d/1pSGNEYEJkci8ely09oc-rdTtnI2ljeqE/preview, name- ATOC Week#5Part3.mp4, duration- 00:53;
+Video: link- https://drive.google.com/file/d/1NJH2YpnIsmDwipOJSgILBo_Ta0u6klH4/preview, name- ATOC Week#5Part4.mp4, duration- 00:02;
+Topics: Research Methods, Minimization of DFAs;
+Note: heading- Presentation in next class;</t>
+  </si>
+  <si>
     <t>Topic: name- Mid Term Exam, lectures- , duration-  14 Mar | 11:00-12:30;
 Assignment: name- Course for Mid Term, img- /STQA/course.jpeg;
+Assignment: name- Paper pattern, img- /STQA/pattern.jpeg;
+Assignment: name- Advise from sir regarding paper, img- /STQA/advise.jpeg;
 Slides: slide- Chapter1.pptx;
 Slides: slide- Chapter2.pptx;
 Slides: slide- Chapter3.ppt;
 Slides: slide- Paper No 1.pdf;
 Slides: slide- Paper No 2.pdf;
 Slides: slide- Paper No 3.pdf;
+Slides: slide- Paper No 4.pdf;
+Slides: slide- Paper No 5.pdf;
 Note: heading- Prepare all lectures pasted above. Must read book. I do not have yet. I will share as I get it.;</t>
-  </si>
-  <si>
-    <t>Topic: name- Mid Term Exam, lectures- , duration-  13 Mar | 15:00-16:30;
-Assignment: name- Course for Mid Term, img- /ATOC/Course.jpeg;
-Slides: slide- Course.pdf;
-Slides: slide- Lec1.pdf;
-Note: heading- Watch all lectures taught in class to prepare for exams;</t>
   </si>
 </sst>
 </file>
@@ -1108,8 +1117,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05FB8366-CFB7-BD41-BAF1-2BC53FC93C19}">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G9" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="C5" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1202,7 +1211,7 @@
         <v>50</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="H3" s="14" t="s">
         <v>83</v>
@@ -1228,13 +1237,13 @@
       </c>
       <c r="F4" s="14"/>
       <c r="G4" s="14" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="H4" s="15" t="s">
         <v>85</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="N4" s="6"/>
     </row>
@@ -1253,17 +1262,17 @@
         <v>32</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="H5" s="15" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="N5" s="5"/>
     </row>
-    <row r="6" spans="1:14" ht="238" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" ht="323" x14ac:dyDescent="0.2">
       <c r="A6" s="8">
         <v>43739</v>
       </c>
@@ -1278,13 +1287,13 @@
         <v>34</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="H6" s="15" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="N6" s="5"/>
     </row>
@@ -1304,10 +1313,10 @@
       </c>
       <c r="F7" s="10"/>
       <c r="G7" s="14" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="N7" s="5"/>
     </row>
@@ -1327,13 +1336,13 @@
       </c>
       <c r="F8" s="10"/>
       <c r="G8" s="14" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="H8" s="14" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="409.6" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A9" s="8">
         <v>43775</v>
       </c>
@@ -1348,7 +1357,7 @@
         <v>53</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="238" x14ac:dyDescent="0.2">

</xml_diff>